<commit_message>
bajas retro y forzar p8 con fecha
</commit_message>
<xml_diff>
--- a/cermi.xlsx
+++ b/cermi.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moree\Desktop\super-herramientas-redles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emore\Desktop\super-herramientas-redles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BD463CB-E2F5-4768-B8DA-6D19C49391EF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="20535" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="20535" windowHeight="15270"/>
   </bookViews>
   <sheets>
     <sheet name="datos" sheetId="1" r:id="rId1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>nroformulario</t>
   </si>
@@ -88,16 +87,19 @@
     <t>Tipo Residencia</t>
   </si>
   <si>
-    <t>falldah@gmail.com</t>
-  </si>
-  <si>
     <t>nromigracion</t>
+  </si>
+  <si>
+    <t>souhaiboudiedhou@gmail.com</t>
+  </si>
+  <si>
+    <t>ayibsene532@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\ mmm\ yyyy"/>
   </numFmts>
@@ -239,6 +241,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -248,12 +251,11 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+    <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal_Hoja3" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal_Hoja3" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -564,14 +566,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
@@ -590,7 +592,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -607,22 +609,22 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>20050444</v>
+        <v>20000798</v>
       </c>
       <c r="B2">
-        <v>20201019</v>
+        <v>20220107</v>
       </c>
       <c r="C2">
-        <v>80000000</v>
+        <v>89113717</v>
       </c>
       <c r="D2">
-        <v>20629540637</v>
+        <v>23630258189</v>
       </c>
       <c r="E2">
         <v>5</v>
       </c>
-      <c r="F2" s="11" t="s">
-        <v>20</v>
+      <c r="F2" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="G2">
         <v>2</v>
@@ -630,44 +632,41 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>21050441</v>
+        <v>20000799</v>
       </c>
       <c r="B3">
-        <v>20210428</v>
+        <v>20211222</v>
       </c>
       <c r="C3">
-        <v>89009419</v>
+        <v>89101816</v>
       </c>
       <c r="D3">
-        <v>20629540637</v>
+        <v>20627934867</v>
       </c>
       <c r="E3">
         <v>5</v>
       </c>
       <c r="F3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G3">
         <v>2</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{DBC38274-C6CA-43B5-AAF1-1D25EEA46B2E}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="38" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30" bestFit="1" customWidth="1"/>
@@ -712,24 +711,24 @@
       <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="11" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
-      <c r="B6" s="10"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="10"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="11"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="11"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>

</xml_diff>